<commit_message>
update test file for occuring panic
</commit_message>
<xml_diff>
--- a/testdata/dump.xlsx
+++ b/testdata/dump.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED280EF-1C1A-4A0E-A27B-CBEA15767006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1534EE-9018-4ACE-B24B-26F25D69DD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-10910" windowWidth="38620" windowHeight="21360" tabRatio="825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="会社" sheetId="89" r:id="rId1"/>
@@ -15167,7 +15167,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F818B3D-F701-434C-A255-6A91A94F7231}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -15364,6 +15364,15 @@
         <v>14</v>
       </c>
     </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="12"/>
   <conditionalFormatting sqref="B5:D5 E5:G9 B8:C9">

</xml_diff>